<commit_message>
updated title in csv and xlsx files for OMAP 16 and 25
</commit_message>
<xml_diff>
--- a/digital-objects/omap/16-lung-codex/v1.1/raw/omap-16-lung-cell-codex.xlsx
+++ b/digital-objects/omap/16-lung-codex/v1.1/raw/omap-16-lung-cell-codex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishi/codeBase/CNS/hra-kg/digital-objects/omap/16-lung-codex/v1.1/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CCB8CD-BC14-D742-B728-6B638A41F80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C159EB4C-60D6-624A-9FC0-BC271F381F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39400" yWindow="4940" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="322">
-  <si>
-    <t>OMAP-16: Organ Mapping Antibody Panel (OMAP) for Multiplexed Antibody-Based Imaging of Lung with CODEX</t>
-  </si>
   <si>
     <t>Author Name(s):</t>
   </si>
@@ -987,6 +984,9 @@
   <si>
     <t>v1.1</t>
   </si>
+  <si>
+    <t>OMAP-16 Organ Mapping Antibody Panel (OMAP) for Multiplexed Antibody-Based Imaging of Human Lung with CODEX</t>
+  </si>
 </sst>
 </file>
 
@@ -1511,9 +1511,7 @@
   </sheetPr>
   <dimension ref="A1:AT1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1524,7 +1522,7 @@
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>321</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1622,10 +1620,10 @@
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>2</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1674,10 +1672,10 @@
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>4</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1726,10 +1724,10 @@
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>6</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="7"/>
@@ -1778,10 +1776,10 @@
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>8</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="7"/>
@@ -1830,10 +1828,10 @@
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>10</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1882,10 +1880,10 @@
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>12</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1934,7 +1932,7 @@
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="14">
         <v>45823</v>
@@ -1986,10 +1984,10 @@
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -2038,82 +2036,82 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="C11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="D11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="E11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="G11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="H11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="I11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="J11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="L11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="M11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="N11" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="N11" s="16" t="s">
+      <c r="O11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="O11" s="16" t="s">
+      <c r="P11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="Q11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="Q11" s="16" t="s">
+      <c r="R11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="R11" s="16" t="s">
+      <c r="S11" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="S11" s="16" t="s">
+      <c r="T11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="T11" s="16" t="s">
+      <c r="U11" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="U11" s="18" t="s">
+      <c r="V11" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="V11" s="18" t="s">
+      <c r="W11" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="W11" s="16" t="s">
+      <c r="X11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="X11" s="16" t="s">
+      <c r="Y11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="Y11" s="16" t="s">
+      <c r="Z11" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="Z11" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="AA11" s="19"/>
       <c r="AB11" s="19"/>
@@ -2138,80 +2136,80 @@
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="E12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="I12" s="22" t="s">
         <v>48</v>
-      </c>
-      <c r="I12" s="22" t="s">
-        <v>49</v>
       </c>
       <c r="J12" s="9">
         <v>4250021</v>
       </c>
       <c r="K12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" s="22" t="s">
         <v>50</v>
-      </c>
-      <c r="L12" s="22" t="s">
-        <v>51</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="23">
         <v>200</v>
       </c>
       <c r="O12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="P12" s="9" t="s">
+      <c r="Q12" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="Q12" s="9" t="s">
+      <c r="R12" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R12" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S12" s="9">
         <v>10</v>
       </c>
       <c r="T12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U12" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U12" s="24" t="s">
+      <c r="V12" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="W12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="X12" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="V12" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="W12" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="X12" s="9" t="s">
+      <c r="Y12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Y12" s="9" t="s">
+      <c r="Z12" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z12" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
@@ -2236,80 +2234,80 @@
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="E13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="9" t="s">
+      <c r="I13" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="J13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="K13" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="L13" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="23">
         <v>100</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P13" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R13" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R13" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S13" s="9">
         <v>3</v>
       </c>
       <c r="T13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U13" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U13" s="24" t="s">
-        <v>57</v>
-      </c>
       <c r="V13" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="X13" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="X13" s="9" t="s">
-        <v>71</v>
-      </c>
       <c r="Y13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z13" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z13" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
@@ -2334,31 +2332,31 @@
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="E14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>75</v>
-      </c>
       <c r="I14" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J14" s="9">
         <v>4250019</v>
@@ -2367,47 +2365,47 @@
         <v>220718025</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M14" s="6"/>
       <c r="N14" s="23">
         <v>200</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R14" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R14" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S14" s="9">
         <v>1</v>
       </c>
       <c r="T14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U14" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U14" s="24" t="s">
-        <v>57</v>
-      </c>
       <c r="V14" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W14" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X14" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Y14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z14" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z14" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
@@ -2432,31 +2430,31 @@
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="D15" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="E15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>82</v>
-      </c>
       <c r="I15" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J15" s="9">
         <v>4450049</v>
@@ -2465,47 +2463,47 @@
         <v>230309013</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P15" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="O15" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="P15" s="9" t="s">
-        <v>84</v>
-      </c>
       <c r="Q15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R15" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R15" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S15" s="9">
         <v>4</v>
       </c>
       <c r="T15" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="U15" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="V15" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="W15" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="X15" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="U15" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="V15" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="W15" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="X15" s="9" t="s">
-        <v>86</v>
-      </c>
       <c r="Y15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z15" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z15" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
@@ -2530,78 +2528,78 @@
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="E16" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="G16" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="K16" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="K16" s="9" t="s">
-        <v>95</v>
-      </c>
       <c r="L16" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P16" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="O16" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="P16" s="9" t="s">
-        <v>97</v>
-      </c>
       <c r="Q16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R16" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R16" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S16" s="9">
         <v>4</v>
       </c>
       <c r="T16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U16" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U16" s="24" t="s">
-        <v>57</v>
-      </c>
       <c r="V16" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W16" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X16" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z16" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z16" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
@@ -2626,80 +2624,80 @@
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="E17" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="F17" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>103</v>
-      </c>
       <c r="I17" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J17" s="9">
         <v>4550118</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M17" s="6"/>
       <c r="N17" s="23">
         <v>200</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R17" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R17" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S17" s="9">
         <v>2</v>
       </c>
       <c r="T17" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="U17" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="V17" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="X17" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="U17" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="V17" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="W17" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="X17" s="9" t="s">
-        <v>107</v>
-      </c>
       <c r="Y17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z17" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z17" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
@@ -2724,80 +2722,80 @@
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="E18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>111</v>
-      </c>
       <c r="I18" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J18" s="9">
         <v>4550113</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M18" s="6"/>
       <c r="N18" s="23">
         <v>200</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R18" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R18" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S18" s="9">
         <v>1</v>
       </c>
       <c r="T18" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="U18" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="V18" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="W18" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="X18" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="U18" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="V18" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="W18" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="X18" s="9" t="s">
-        <v>115</v>
-      </c>
       <c r="Y18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z18" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z18" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
@@ -2822,80 +2820,80 @@
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="E19" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>119</v>
-      </c>
       <c r="I19" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J19" s="27">
         <v>4550121</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M19" s="6"/>
       <c r="N19" s="23">
         <v>200</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P19" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q19" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R19" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R19" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S19" s="9">
         <v>5</v>
       </c>
       <c r="T19" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U19" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V19" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W19" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X19" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Y19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z19" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z19" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
@@ -2920,80 +2918,80 @@
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="E20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H20" s="9" t="s">
+      <c r="I20" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="J20" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="J20" s="28" t="s">
+      <c r="K20" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="K20" s="21" t="s">
-        <v>129</v>
-      </c>
       <c r="L20" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M20" s="6"/>
       <c r="N20" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P20" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="O20" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="P20" s="21" t="s">
-        <v>131</v>
-      </c>
       <c r="Q20" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R20" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R20" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S20" s="9">
         <v>9</v>
       </c>
       <c r="T20" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="U20" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="V20" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="W20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="X20" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="U20" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="V20" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="W20" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="X20" s="9" t="s">
-        <v>133</v>
-      </c>
       <c r="Y20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z20" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z20" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
@@ -3018,80 +3016,80 @@
     </row>
     <row r="21" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="E21" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>137</v>
-      </c>
       <c r="I21" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J21" s="9">
         <v>4550119</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M21" s="6"/>
       <c r="N21" s="23">
         <v>200</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R21" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R21" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S21" s="9">
         <v>3</v>
       </c>
       <c r="T21" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U21" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V21" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W21" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X21" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z21" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z21" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
@@ -3116,80 +3114,80 @@
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="D22" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="E22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>144</v>
-      </c>
       <c r="I22" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J22" s="9">
         <v>4450018</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M22" s="6"/>
       <c r="N22" s="23">
         <v>200</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P22" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R22" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R22" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S22" s="9">
         <v>2</v>
       </c>
       <c r="T22" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U22" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V22" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W22" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X22" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Y22" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z22" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z22" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
@@ -3214,80 +3212,80 @@
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="D23" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="E23" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="I23" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J23" s="9">
         <v>4450017</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M23" s="6"/>
       <c r="N23" s="23">
         <v>200</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P23" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R23" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R23" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S23" s="9">
         <v>3</v>
       </c>
       <c r="T23" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U23" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V23" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W23" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X23" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Y23" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z23" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z23" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
@@ -3312,78 +3310,78 @@
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="D24" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="D24" s="21" t="s">
-        <v>157</v>
-      </c>
       <c r="E24" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="J24" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="K24" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="K24" s="9" t="s">
-        <v>160</v>
-      </c>
       <c r="L24" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M24" s="6"/>
       <c r="N24" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P24" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R24" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R24" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S24" s="9">
         <v>5</v>
       </c>
       <c r="T24" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U24" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V24" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W24" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X24" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Y24" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z24" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z24" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
@@ -3408,78 +3406,78 @@
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="E25" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>166</v>
-      </c>
       <c r="F25" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="J25" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="K25" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="K25" s="9" t="s">
-        <v>169</v>
-      </c>
       <c r="L25" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M25" s="6"/>
       <c r="N25" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="O25" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P25" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="O25" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="P25" s="9" t="s">
-        <v>171</v>
-      </c>
       <c r="Q25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R25" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R25" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S25" s="9">
         <v>6</v>
       </c>
       <c r="T25" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U25" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V25" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W25" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X25" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y25" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z25" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z25" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
@@ -3504,80 +3502,80 @@
     </row>
     <row r="26" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="E26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>176</v>
-      </c>
       <c r="I26" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J26" s="9">
         <v>4450020</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="23">
         <v>200</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q26" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R26" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R26" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S26" s="9">
         <v>1</v>
       </c>
       <c r="T26" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U26" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W26" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X26" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Y26" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z26" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z26" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
@@ -3602,80 +3600,80 @@
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="D27" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="E27" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>182</v>
-      </c>
       <c r="I27" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J27" s="9">
         <v>4250012</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M27" s="6"/>
       <c r="N27" s="23">
         <v>200</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P27" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R27" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R27" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S27" s="9">
         <v>2</v>
       </c>
       <c r="T27" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U27" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U27" s="24" t="s">
-        <v>57</v>
-      </c>
       <c r="V27" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W27" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X27" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Y27" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z27" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z27" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
@@ -3700,31 +3698,31 @@
     </row>
     <row r="28" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="D28" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="E28" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>189</v>
-      </c>
       <c r="I28" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J28" s="29">
         <v>240017</v>
@@ -3733,47 +3731,47 @@
         <v>230502016</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M28" s="6"/>
       <c r="N28" s="23">
         <v>200</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Q28" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R28" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R28" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S28" s="9">
         <v>4</v>
       </c>
       <c r="T28" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U28" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V28" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W28" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X28" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Y28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z28" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z28" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
@@ -3798,80 +3796,80 @@
     </row>
     <row r="29" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="D29" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="E29" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H29" s="9" t="s">
+      <c r="I29" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J29" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="I29" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="J29" s="21" t="s">
+      <c r="K29" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="K29" s="21" t="s">
-        <v>197</v>
-      </c>
       <c r="L29" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M29" s="6"/>
       <c r="N29" s="23">
         <v>100</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R29" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R29" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S29" s="9">
         <v>7</v>
       </c>
       <c r="T29" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U29" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W29" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X29" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Y29" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z29" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z29" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
@@ -3896,80 +3894,80 @@
     </row>
     <row r="30" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="D30" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="E30" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H30" s="9" t="s">
+      <c r="I30" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J30" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="J30" s="30" t="s">
+      <c r="K30" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="K30" s="21" t="s">
-        <v>205</v>
-      </c>
       <c r="L30" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M30" s="6"/>
       <c r="N30" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P30" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q30" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R30" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R30" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S30" s="9">
         <v>10</v>
       </c>
       <c r="T30" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U30" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W30" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X30" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z30" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z30" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
@@ -3994,80 +3992,80 @@
     </row>
     <row r="31" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="D31" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="E31" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="F31" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="F31" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H31" s="9" t="s">
+      <c r="I31" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J31" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="J31" s="9" t="s">
+      <c r="K31" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="K31" s="9" t="s">
-        <v>214</v>
-      </c>
       <c r="L31" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M31" s="6"/>
       <c r="N31" s="23">
         <v>1000</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P31" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q31" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R31" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R31" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S31" s="9">
         <v>6</v>
       </c>
       <c r="T31" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U31" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U31" s="24" t="s">
-        <v>57</v>
-      </c>
       <c r="V31" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W31" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X31" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Y31" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z31" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z31" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
@@ -4092,80 +4090,80 @@
     </row>
     <row r="32" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="D32" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="E32" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>220</v>
-      </c>
       <c r="I32" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J32" s="9">
         <v>4450047</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M32" s="6"/>
       <c r="N32" s="23">
         <v>200</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P32" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q32" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R32" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R32" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S32" s="9">
         <v>3</v>
       </c>
       <c r="T32" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U32" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U32" s="24" t="s">
-        <v>57</v>
-      </c>
       <c r="V32" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W32" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X32" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Y32" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z32" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z32" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
@@ -4190,80 +4188,80 @@
     </row>
     <row r="33" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="D33" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="E33" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F33" s="9" t="s">
+      <c r="G33" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="G33" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H33" s="9" t="s">
+      <c r="I33" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J33" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="I33" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="J33" s="9" t="s">
+      <c r="K33" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="K33" s="9" t="s">
-        <v>230</v>
-      </c>
       <c r="L33" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M33" s="6"/>
       <c r="N33" s="23">
         <v>100</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P33" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q33" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R33" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R33" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S33" s="9">
         <v>5</v>
       </c>
       <c r="T33" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U33" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U33" s="24" t="s">
-        <v>57</v>
-      </c>
       <c r="V33" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W33" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X33" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Y33" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z33" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z33" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA33" s="6"/>
       <c r="AB33" s="6"/>
@@ -4288,80 +4286,80 @@
     </row>
     <row r="34" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="D34" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="E34" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H34" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>236</v>
-      </c>
       <c r="I34" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J34" s="9">
         <v>4250079</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M34" s="6"/>
       <c r="N34" s="23">
         <v>200</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P34" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Q34" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R34" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R34" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S34" s="9">
         <v>7</v>
       </c>
       <c r="T34" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U34" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U34" s="24" t="s">
-        <v>57</v>
-      </c>
       <c r="V34" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W34" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X34" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Y34" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z34" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z34" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA34" s="6"/>
       <c r="AB34" s="6"/>
@@ -4386,80 +4384,80 @@
     </row>
     <row r="35" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="D35" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="E35" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H35" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>243</v>
-      </c>
       <c r="I35" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J35" s="9">
         <v>4550122</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L35" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M35" s="6"/>
       <c r="N35" s="23">
         <v>200</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P35" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Q35" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R35" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R35" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S35" s="9">
         <v>8</v>
       </c>
       <c r="T35" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U35" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W35" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X35" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Y35" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z35" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z35" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA35" s="6"/>
       <c r="AB35" s="6"/>
@@ -4484,80 +4482,80 @@
     </row>
     <row r="36" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="D36" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="E36" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>249</v>
-      </c>
       <c r="I36" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J36" s="9">
         <v>4450090</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L36" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M36" s="6"/>
       <c r="N36" s="23">
         <v>200</v>
       </c>
       <c r="O36" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q36" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R36" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R36" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S36" s="9">
         <v>8</v>
       </c>
       <c r="T36" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U36" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W36" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X36" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y36" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z36" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z36" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA36" s="6"/>
       <c r="AB36" s="6"/>
@@ -4582,80 +4580,80 @@
     </row>
     <row r="37" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="D37" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="E37" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>255</v>
-      </c>
       <c r="I37" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J37" s="9">
         <v>4550071</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L37" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M37" s="6"/>
       <c r="N37" s="23">
         <v>200</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P37" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q37" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R37" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R37" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S37" s="9">
         <v>7</v>
       </c>
       <c r="T37" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U37" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V37" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W37" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X37" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Y37" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z37" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z37" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA37" s="6"/>
       <c r="AB37" s="6"/>
@@ -4680,80 +4678,80 @@
     </row>
     <row r="38" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="D38" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="E38" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F38" s="9" t="s">
+      <c r="G38" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H38" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="G38" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>263</v>
-      </c>
       <c r="I38" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J38" s="21">
         <v>4550114</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L38" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M38" s="6"/>
       <c r="N38" s="23">
         <v>200</v>
       </c>
       <c r="O38" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P38" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q38" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R38" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R38" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S38" s="9">
         <v>6</v>
       </c>
       <c r="T38" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U38" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V38" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W38" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X38" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Y38" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z38" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z38" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA38" s="6"/>
       <c r="AB38" s="6"/>
@@ -4778,31 +4776,31 @@
     </row>
     <row r="39" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="C39" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="D39" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="E39" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="E39" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="F39" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H39" s="21" t="s">
-        <v>270</v>
-      </c>
       <c r="I39" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J39" s="21">
         <v>4250083</v>
@@ -4811,47 +4809,47 @@
         <v>230518016</v>
       </c>
       <c r="L39" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M39" s="6"/>
       <c r="N39" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O39" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P39" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q39" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R39" s="21" t="s">
         <v>54</v>
-      </c>
-      <c r="R39" s="21" t="s">
-        <v>55</v>
       </c>
       <c r="S39" s="21">
         <v>8</v>
       </c>
       <c r="T39" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U39" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U39" s="24" t="s">
-        <v>57</v>
-      </c>
       <c r="V39" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W39" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X39" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Y39" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z39" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z39" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA39" s="6"/>
       <c r="AB39" s="6"/>
@@ -4876,78 +4874,78 @@
     </row>
     <row r="40" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="D40" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="D40" s="21" t="s">
-        <v>275</v>
-      </c>
       <c r="E40" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="G40" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="J40" s="21" t="s">
         <v>276</v>
       </c>
-      <c r="J40" s="21" t="s">
+      <c r="K40" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="K40" s="21" t="s">
-        <v>278</v>
-      </c>
       <c r="L40" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M40" s="6"/>
       <c r="N40" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O40" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Q40" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R40" s="21" t="s">
         <v>54</v>
-      </c>
-      <c r="R40" s="21" t="s">
-        <v>55</v>
       </c>
       <c r="S40" s="21">
         <v>9</v>
       </c>
       <c r="T40" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U40" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V40" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W40" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X40" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Y40" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z40" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z40" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA40" s="6"/>
       <c r="AB40" s="6"/>
@@ -4972,80 +4970,80 @@
     </row>
     <row r="41" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="C41" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="D41" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="E41" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H41" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="E41" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F41" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H41" s="21" t="s">
+      <c r="I41" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="J41" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="I41" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="J41" s="21" t="s">
+      <c r="K41" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="K41" s="21" t="s">
-        <v>285</v>
-      </c>
       <c r="L41" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M41" s="6"/>
       <c r="N41" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="O41" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P41" s="21" t="s">
         <v>286</v>
       </c>
-      <c r="O41" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="P41" s="21" t="s">
-        <v>287</v>
-      </c>
       <c r="Q41" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R41" s="21" t="s">
         <v>54</v>
-      </c>
-      <c r="R41" s="21" t="s">
-        <v>55</v>
       </c>
       <c r="S41" s="21">
         <v>9</v>
       </c>
       <c r="T41" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U41" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U41" s="24" t="s">
-        <v>57</v>
-      </c>
       <c r="V41" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W41" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X41" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Y41" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z41" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z41" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA41" s="6"/>
       <c r="AB41" s="6"/>
@@ -5070,80 +5068,80 @@
     </row>
     <row r="42" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="C42" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="D42" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="E42" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="E42" s="21" t="s">
-        <v>292</v>
-      </c>
       <c r="F42" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G42" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="H42" s="21">
         <v>394324</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J42" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="K42" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="K42" s="21" t="s">
-        <v>294</v>
-      </c>
       <c r="L42" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M42" s="6"/>
       <c r="N42" s="32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O42" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P42" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Q42" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R42" s="21" t="s">
         <v>54</v>
-      </c>
-      <c r="R42" s="21" t="s">
-        <v>55</v>
       </c>
       <c r="S42" s="21">
         <v>10</v>
       </c>
       <c r="T42" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U42" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V42" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W42" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X42" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="Y42" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z42" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z42" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA42" s="6"/>
       <c r="AB42" s="6"/>
@@ -5168,80 +5166,80 @@
     </row>
     <row r="43" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="C43" s="21" t="s">
         <v>297</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="D43" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="E43" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="F43" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H43" s="33" t="s">
         <v>300</v>
       </c>
-      <c r="F43" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H43" s="33" t="s">
+      <c r="I43" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J43" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="I43" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="J43" s="21" t="s">
+      <c r="K43" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="K43" s="21" t="s">
-        <v>303</v>
-      </c>
       <c r="L43" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M43" s="6"/>
       <c r="N43" s="32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O43" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P43" s="25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Q43" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R43" s="21" t="s">
         <v>54</v>
-      </c>
-      <c r="R43" s="21" t="s">
-        <v>55</v>
       </c>
       <c r="S43" s="21">
         <v>11</v>
       </c>
       <c r="T43" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U43" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="U43" s="24" t="s">
-        <v>57</v>
-      </c>
       <c r="V43" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W43" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X43" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Y43" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z43" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z43" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA43" s="6"/>
       <c r="AB43" s="6"/>
@@ -5266,80 +5264,80 @@
     </row>
     <row r="44" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" s="21" t="s">
+        <v>305</v>
+      </c>
+      <c r="C44" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="D44" s="21" t="s">
         <v>307</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="E44" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H44" s="21" t="s">
         <v>308</v>
       </c>
-      <c r="E44" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F44" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H44" s="21" t="s">
+      <c r="I44" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J44" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="I44" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="J44" s="21" t="s">
+      <c r="K44" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="K44" s="21" t="s">
-        <v>311</v>
-      </c>
       <c r="L44" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M44" s="6"/>
       <c r="N44" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O44" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P44" s="21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Q44" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R44" s="21" t="s">
         <v>54</v>
-      </c>
-      <c r="R44" s="21" t="s">
-        <v>55</v>
       </c>
       <c r="S44" s="21">
         <v>11</v>
       </c>
       <c r="T44" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U44" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V44" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W44" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X44" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Y44" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z44" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z44" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA44" s="6"/>
       <c r="AB44" s="6"/>
@@ -5364,78 +5362,78 @@
     </row>
     <row r="45" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="C45" s="35" t="s">
         <v>314</v>
       </c>
-      <c r="C45" s="35" t="s">
+      <c r="D45" s="21" t="s">
         <v>315</v>
       </c>
-      <c r="D45" s="21" t="s">
-        <v>316</v>
-      </c>
       <c r="E45" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F45" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G45" s="21" t="s">
         <v>91</v>
-      </c>
-      <c r="G45" s="21" t="s">
-        <v>92</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J45" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="K45" s="21" t="s">
         <v>317</v>
       </c>
-      <c r="K45" s="21" t="s">
-        <v>318</v>
-      </c>
       <c r="L45" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M45" s="6"/>
       <c r="N45" s="21">
         <v>200</v>
       </c>
       <c r="O45" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P45" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q45" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R45" s="21" t="s">
         <v>54</v>
-      </c>
-      <c r="R45" s="21" t="s">
-        <v>55</v>
       </c>
       <c r="S45" s="21">
         <v>12</v>
       </c>
       <c r="T45" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U45" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="U45" s="36" t="s">
-        <v>57</v>
-      </c>
       <c r="V45" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W45" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X45" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Y45" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z45" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="Z45" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="AA45" s="6"/>
       <c r="AB45" s="6"/>

</xml_diff>

<commit_message>
created new version for omap 16 and 25
</commit_message>
<xml_diff>
--- a/digital-objects/omap/16-lung-codex/v1.1/raw/omap-16-lung-cell-codex.xlsx
+++ b/digital-objects/omap/16-lung-codex/v1.1/raw/omap-16-lung-cell-codex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishi/codeBase/CNS/hra-kg/digital-objects/omap/16-lung-codex/v1.1/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C159EB4C-60D6-624A-9FC0-BC271F381F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF17769B-DD00-7B49-A715-FE17EA0757A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39400" yWindow="4940" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -985,7 +985,7 @@
     <t>v1.1</t>
   </si>
   <si>
-    <t>OMAP-16 Organ Mapping Antibody Panel (OMAP) for Multiplexed Antibody-Based Imaging of Human Lung with CODEX</t>
+    <t>OMAP-16: Organ Mapping Antibody Panel (OMAP) for Multiplexed Antibody-Based Imaging of Lung with CODEX</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
replaced xlsx files from main into develop from OMAP 16 and 25
</commit_message>
<xml_diff>
--- a/digital-objects/omap/16-lung-codex/v1.1/raw/omap-16-lung-cell-codex.xlsx
+++ b/digital-objects/omap/16-lung-codex/v1.1/raw/omap-16-lung-cell-codex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishi/codeBase/CNS/hra-kg/digital-objects/omap/16-lung-codex/v1.1/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF17769B-DD00-7B49-A715-FE17EA0757A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CCB8CD-BC14-D742-B728-6B638A41F80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39400" yWindow="4940" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="322">
+  <si>
+    <t>OMAP-16: Organ Mapping Antibody Panel (OMAP) for Multiplexed Antibody-Based Imaging of Lung with CODEX</t>
+  </si>
   <si>
     <t>Author Name(s):</t>
   </si>
@@ -984,9 +987,6 @@
   <si>
     <t>v1.1</t>
   </si>
-  <si>
-    <t>OMAP-16: Organ Mapping Antibody Panel (OMAP) for Multiplexed Antibody-Based Imaging of Lung with CODEX</t>
-  </si>
 </sst>
 </file>
 
@@ -1511,7 +1511,9 @@
   </sheetPr>
   <dimension ref="A1:AT1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1522,7 +1524,7 @@
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>321</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1620,10 +1622,10 @@
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1672,10 +1674,10 @@
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1724,10 +1726,10 @@
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="7"/>
@@ -1776,10 +1778,10 @@
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="7"/>
@@ -1828,10 +1830,10 @@
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1880,10 +1882,10 @@
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1932,7 +1934,7 @@
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="14">
         <v>45823</v>
@@ -1984,10 +1986,10 @@
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -2036,82 +2038,82 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N11" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q11" s="16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R11" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S11" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T11" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U11" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V11" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W11" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X11" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y11" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z11" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA11" s="19"/>
       <c r="AB11" s="19"/>
@@ -2136,80 +2138,80 @@
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J12" s="9">
         <v>4250021</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="23">
         <v>200</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R12" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S12" s="9">
         <v>10</v>
       </c>
       <c r="T12" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U12" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V12" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W12" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X12" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Y12" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z12" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
@@ -2234,80 +2236,80 @@
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="23">
         <v>100</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P13" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R13" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S13" s="9">
         <v>3</v>
       </c>
       <c r="T13" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U13" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V13" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W13" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X13" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Y13" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z13" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
@@ -2332,31 +2334,31 @@
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J14" s="9">
         <v>4250019</v>
@@ -2365,47 +2367,47 @@
         <v>220718025</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M14" s="6"/>
       <c r="N14" s="23">
         <v>200</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S14" s="9">
         <v>1</v>
       </c>
       <c r="T14" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U14" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V14" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W14" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X14" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Y14" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z14" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
@@ -2430,31 +2432,31 @@
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J15" s="9">
         <v>4450049</v>
@@ -2463,47 +2465,47 @@
         <v>230309013</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R15" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S15" s="9">
         <v>4</v>
       </c>
       <c r="T15" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U15" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V15" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W15" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X15" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Y15" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z15" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
@@ -2528,78 +2530,78 @@
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L16" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R16" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S16" s="9">
         <v>4</v>
       </c>
       <c r="T16" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U16" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V16" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W16" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X16" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Y16" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z16" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
@@ -2624,80 +2626,80 @@
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J17" s="9">
         <v>4550118</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M17" s="6"/>
       <c r="N17" s="23">
         <v>200</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R17" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S17" s="9">
         <v>2</v>
       </c>
       <c r="T17" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="U17" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V17" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W17" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X17" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Y17" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z17" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
@@ -2722,80 +2724,80 @@
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J18" s="9">
         <v>4550113</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M18" s="6"/>
       <c r="N18" s="23">
         <v>200</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S18" s="9">
         <v>1</v>
       </c>
       <c r="T18" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="U18" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V18" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W18" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X18" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Y18" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z18" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
@@ -2820,80 +2822,80 @@
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J19" s="27">
         <v>4550121</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M19" s="6"/>
       <c r="N19" s="23">
         <v>200</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P19" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S19" s="9">
         <v>5</v>
       </c>
       <c r="T19" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="U19" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V19" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W19" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X19" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Y19" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z19" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA19" s="6"/>
       <c r="AB19" s="6"/>
@@ -2918,80 +2920,80 @@
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J20" s="28" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K20" s="21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L20" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M20" s="6"/>
       <c r="N20" s="23" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P20" s="21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S20" s="9">
         <v>9</v>
       </c>
       <c r="T20" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="U20" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V20" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W20" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X20" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Y20" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z20" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
@@ -3016,80 +3018,80 @@
     </row>
     <row r="21" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J21" s="9">
         <v>4550119</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M21" s="6"/>
       <c r="N21" s="23">
         <v>200</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R21" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S21" s="9">
         <v>3</v>
       </c>
       <c r="T21" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="U21" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V21" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W21" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X21" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="Y21" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z21" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
@@ -3114,80 +3116,80 @@
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J22" s="9">
         <v>4450018</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M22" s="6"/>
       <c r="N22" s="23">
         <v>200</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P22" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S22" s="9">
         <v>2</v>
       </c>
       <c r="T22" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U22" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V22" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W22" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X22" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Y22" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z22" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA22" s="6"/>
       <c r="AB22" s="6"/>
@@ -3212,80 +3214,80 @@
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J23" s="9">
         <v>4450017</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M23" s="6"/>
       <c r="N23" s="23">
         <v>200</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P23" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R23" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S23" s="9">
         <v>3</v>
       </c>
       <c r="T23" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U23" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V23" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W23" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X23" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="Y23" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z23" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA23" s="6"/>
       <c r="AB23" s="6"/>
@@ -3310,78 +3312,78 @@
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M24" s="6"/>
       <c r="N24" s="23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P24" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R24" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S24" s="9">
         <v>5</v>
       </c>
       <c r="T24" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U24" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V24" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W24" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X24" s="9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="Y24" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z24" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
@@ -3406,78 +3408,78 @@
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="L25" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M25" s="6"/>
       <c r="N25" s="23" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P25" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R25" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S25" s="9">
         <v>6</v>
       </c>
       <c r="T25" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U25" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V25" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W25" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X25" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Y25" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z25" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
@@ -3502,80 +3504,80 @@
     </row>
     <row r="26" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J26" s="9">
         <v>4450020</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="23">
         <v>200</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R26" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S26" s="9">
         <v>1</v>
       </c>
       <c r="T26" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U26" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W26" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X26" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Y26" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z26" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
@@ -3600,80 +3602,80 @@
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J27" s="9">
         <v>4250012</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M27" s="6"/>
       <c r="N27" s="23">
         <v>200</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P27" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R27" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S27" s="9">
         <v>2</v>
       </c>
       <c r="T27" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U27" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V27" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W27" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X27" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Y27" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z27" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
@@ -3698,31 +3700,31 @@
     </row>
     <row r="28" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J28" s="29">
         <v>240017</v>
@@ -3731,47 +3733,47 @@
         <v>230502016</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M28" s="6"/>
       <c r="N28" s="23">
         <v>200</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R28" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S28" s="9">
         <v>4</v>
       </c>
       <c r="T28" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="U28" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V28" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W28" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X28" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="Y28" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z28" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
@@ -3796,80 +3798,80 @@
     </row>
     <row r="29" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J29" s="21" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K29" s="21" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M29" s="6"/>
       <c r="N29" s="23">
         <v>100</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R29" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S29" s="9">
         <v>7</v>
       </c>
       <c r="T29" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U29" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W29" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X29" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="Y29" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z29" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
@@ -3894,80 +3896,80 @@
     </row>
     <row r="30" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J30" s="30" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M30" s="6"/>
       <c r="N30" s="23" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P30" s="21" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="Q30" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R30" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S30" s="9">
         <v>10</v>
       </c>
       <c r="T30" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="U30" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W30" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X30" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="Y30" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z30" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
@@ -3992,80 +3994,80 @@
     </row>
     <row r="31" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="L31" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M31" s="6"/>
       <c r="N31" s="23">
         <v>1000</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P31" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="Q31" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R31" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S31" s="9">
         <v>6</v>
       </c>
       <c r="T31" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U31" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V31" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W31" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X31" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="Y31" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z31" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
@@ -4090,80 +4092,80 @@
     </row>
     <row r="32" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J32" s="9">
         <v>4450047</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M32" s="6"/>
       <c r="N32" s="23">
         <v>200</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P32" s="21" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="Q32" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R32" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S32" s="9">
         <v>3</v>
       </c>
       <c r="T32" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U32" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V32" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W32" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X32" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="Y32" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z32" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
@@ -4188,80 +4190,80 @@
     </row>
     <row r="33" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M33" s="6"/>
       <c r="N33" s="23">
         <v>100</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P33" s="9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Q33" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R33" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S33" s="9">
         <v>5</v>
       </c>
       <c r="T33" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U33" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V33" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W33" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X33" s="9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="Y33" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z33" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA33" s="6"/>
       <c r="AB33" s="6"/>
@@ -4286,80 +4288,80 @@
     </row>
     <row r="34" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J34" s="9">
         <v>4250079</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M34" s="6"/>
       <c r="N34" s="23">
         <v>200</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P34" s="9" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="Q34" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R34" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S34" s="9">
         <v>7</v>
       </c>
       <c r="T34" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U34" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V34" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W34" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X34" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="Y34" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z34" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA34" s="6"/>
       <c r="AB34" s="6"/>
@@ -4384,80 +4386,80 @@
     </row>
     <row r="35" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J35" s="9">
         <v>4550122</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L35" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M35" s="6"/>
       <c r="N35" s="23">
         <v>200</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P35" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="Q35" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R35" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S35" s="9">
         <v>8</v>
       </c>
       <c r="T35" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="U35" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W35" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X35" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Y35" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z35" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA35" s="6"/>
       <c r="AB35" s="6"/>
@@ -4482,80 +4484,80 @@
     </row>
     <row r="36" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J36" s="9">
         <v>4450090</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L36" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M36" s="6"/>
       <c r="N36" s="23">
         <v>200</v>
       </c>
       <c r="O36" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="Q36" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R36" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S36" s="9">
         <v>8</v>
       </c>
       <c r="T36" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U36" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W36" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X36" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="Y36" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z36" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA36" s="6"/>
       <c r="AB36" s="6"/>
@@ -4580,80 +4582,80 @@
     </row>
     <row r="37" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J37" s="9">
         <v>4550071</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="L37" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M37" s="6"/>
       <c r="N37" s="23">
         <v>200</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P37" s="9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="Q37" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R37" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S37" s="9">
         <v>7</v>
       </c>
       <c r="T37" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="U37" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V37" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W37" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X37" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="Y37" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z37" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA37" s="6"/>
       <c r="AB37" s="6"/>
@@ -4678,80 +4680,80 @@
     </row>
     <row r="38" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J38" s="21">
         <v>4550114</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L38" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M38" s="6"/>
       <c r="N38" s="23">
         <v>200</v>
       </c>
       <c r="O38" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P38" s="21" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Q38" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R38" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S38" s="9">
         <v>6</v>
       </c>
       <c r="T38" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="U38" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V38" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W38" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X38" s="9" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="Y38" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z38" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA38" s="6"/>
       <c r="AB38" s="6"/>
@@ -4776,31 +4778,31 @@
     </row>
     <row r="39" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J39" s="21">
         <v>4250083</v>
@@ -4809,47 +4811,47 @@
         <v>230518016</v>
       </c>
       <c r="L39" s="21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M39" s="6"/>
       <c r="N39" s="32" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O39" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P39" s="9" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="Q39" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R39" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S39" s="21">
         <v>8</v>
       </c>
       <c r="T39" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U39" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V39" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W39" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X39" s="9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="Y39" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z39" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA39" s="6"/>
       <c r="AB39" s="6"/>
@@ -4874,78 +4876,78 @@
     </row>
     <row r="40" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="21" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="J40" s="21" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="L40" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M40" s="6"/>
       <c r="N40" s="32" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O40" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="Q40" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R40" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S40" s="21">
         <v>9</v>
       </c>
       <c r="T40" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U40" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V40" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W40" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X40" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="Y40" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z40" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA40" s="6"/>
       <c r="AB40" s="6"/>
@@ -4970,80 +4972,80 @@
     </row>
     <row r="41" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J41" s="21" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="K41" s="21" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="L41" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M41" s="6"/>
       <c r="N41" s="32" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="O41" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P41" s="21" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="Q41" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R41" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S41" s="21">
         <v>9</v>
       </c>
       <c r="T41" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U41" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V41" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W41" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X41" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="Y41" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z41" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA41" s="6"/>
       <c r="AB41" s="6"/>
@@ -5068,80 +5070,80 @@
     </row>
     <row r="42" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H42" s="21">
         <v>394324</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L42" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M42" s="6"/>
       <c r="N42" s="32" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="O42" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P42" s="9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="Q42" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R42" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S42" s="21">
         <v>10</v>
       </c>
       <c r="T42" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U42" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V42" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W42" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X42" s="9" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="Y42" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z42" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA42" s="6"/>
       <c r="AB42" s="6"/>
@@ -5166,80 +5168,80 @@
     </row>
     <row r="43" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H43" s="33" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L43" s="21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M43" s="6"/>
       <c r="N43" s="32" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="O43" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P43" s="25" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="Q43" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R43" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S43" s="21">
         <v>11</v>
       </c>
       <c r="T43" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U43" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V43" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W43" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X43" s="9" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="Y43" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z43" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA43" s="6"/>
       <c r="AB43" s="6"/>
@@ -5264,80 +5266,80 @@
     </row>
     <row r="44" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="L44" s="21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M44" s="6"/>
       <c r="N44" s="32" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O44" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P44" s="21" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="Q44" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R44" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S44" s="21">
         <v>11</v>
       </c>
       <c r="T44" s="21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U44" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V44" s="25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W44" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X44" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="Y44" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z44" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA44" s="6"/>
       <c r="AB44" s="6"/>
@@ -5362,78 +5364,78 @@
     </row>
     <row r="45" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C45" s="35" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G45" s="21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J45" s="21" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L45" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M45" s="6"/>
       <c r="N45" s="21">
         <v>200</v>
       </c>
       <c r="O45" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P45" s="9" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="Q45" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R45" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S45" s="21">
         <v>12</v>
       </c>
       <c r="T45" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U45" s="36" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V45" s="9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W45" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X45" s="9" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="Y45" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z45" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA45" s="6"/>
       <c r="AB45" s="6"/>

</xml_diff>